<commit_message>
wk5 slides files and plan
</commit_message>
<xml_diff>
--- a/xlfiles/Chapter3.xlsx
+++ b/xlfiles/Chapter3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bavanzi/Dropbox/Mac (3)/Documents/GitHub/ACTL20004-ACTL90021-2024/xlfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849FDDE-7618-3944-AA2F-BECAAF490705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AEDF7F-5462-F64A-805B-0E66CD7F20C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{065E86FA-80AD-4F4F-B6B7-2E1659088BBF}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="28720" windowHeight="21580" activeTab="3" xr2:uid="{065E86FA-80AD-4F4F-B6B7-2E1659088BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment data" sheetId="1" r:id="rId1"/>
@@ -2418,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092A182E-02B0-8447-9474-8F02EF93B344}">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -2442,127 +2442,127 @@
         <v>1964</v>
       </c>
       <c r="D3" s="3">
-        <f>C3+1</f>
+        <f t="shared" ref="D3:AH3" si="0">C3+1</f>
         <v>1965</v>
       </c>
       <c r="E3" s="3">
-        <f>D3+1</f>
+        <f t="shared" si="0"/>
         <v>1966</v>
       </c>
       <c r="F3" s="3">
-        <f>E3+1</f>
+        <f t="shared" si="0"/>
         <v>1967</v>
       </c>
       <c r="G3" s="3">
-        <f>F3+1</f>
+        <f t="shared" si="0"/>
         <v>1968</v>
       </c>
       <c r="H3" s="3">
-        <f>G3+1</f>
+        <f t="shared" si="0"/>
         <v>1969</v>
       </c>
       <c r="I3" s="3">
-        <f>H3+1</f>
+        <f t="shared" si="0"/>
         <v>1970</v>
       </c>
       <c r="J3" s="3">
-        <f>I3+1</f>
+        <f t="shared" si="0"/>
         <v>1971</v>
       </c>
       <c r="K3" s="3">
-        <f>J3+1</f>
+        <f t="shared" si="0"/>
         <v>1972</v>
       </c>
       <c r="L3" s="3">
-        <f>K3+1</f>
+        <f t="shared" si="0"/>
         <v>1973</v>
       </c>
       <c r="M3" s="3">
-        <f>L3+1</f>
+        <f t="shared" si="0"/>
         <v>1974</v>
       </c>
       <c r="N3" s="3">
-        <f>M3+1</f>
+        <f t="shared" si="0"/>
         <v>1975</v>
       </c>
       <c r="O3" s="3">
-        <f>N3+1</f>
+        <f t="shared" si="0"/>
         <v>1976</v>
       </c>
       <c r="P3" s="3">
-        <f>O3+1</f>
+        <f t="shared" si="0"/>
         <v>1977</v>
       </c>
       <c r="Q3" s="3">
-        <f>P3+1</f>
+        <f t="shared" si="0"/>
         <v>1978</v>
       </c>
       <c r="R3" s="3">
-        <f>Q3+1</f>
+        <f t="shared" si="0"/>
         <v>1979</v>
       </c>
       <c r="S3" s="3">
-        <f>R3+1</f>
+        <f t="shared" si="0"/>
         <v>1980</v>
       </c>
       <c r="T3" s="3">
-        <f>S3+1</f>
+        <f t="shared" si="0"/>
         <v>1981</v>
       </c>
       <c r="U3" s="3">
-        <f>T3+1</f>
+        <f t="shared" si="0"/>
         <v>1982</v>
       </c>
       <c r="V3" s="3">
-        <f>U3+1</f>
+        <f t="shared" si="0"/>
         <v>1983</v>
       </c>
       <c r="W3" s="3">
-        <f>V3+1</f>
+        <f t="shared" si="0"/>
         <v>1984</v>
       </c>
       <c r="X3" s="3">
-        <f>W3+1</f>
+        <f t="shared" si="0"/>
         <v>1985</v>
       </c>
       <c r="Y3" s="3">
-        <f>X3+1</f>
+        <f t="shared" si="0"/>
         <v>1986</v>
       </c>
       <c r="Z3" s="3">
-        <f>Y3+1</f>
+        <f t="shared" si="0"/>
         <v>1987</v>
       </c>
       <c r="AA3" s="3">
-        <f>Z3+1</f>
+        <f t="shared" si="0"/>
         <v>1988</v>
       </c>
       <c r="AB3" s="3">
-        <f>AA3+1</f>
+        <f t="shared" si="0"/>
         <v>1989</v>
       </c>
       <c r="AC3" s="3">
-        <f>AB3+1</f>
+        <f t="shared" si="0"/>
         <v>1990</v>
       </c>
       <c r="AD3" s="3">
-        <f>AC3+1</f>
+        <f t="shared" si="0"/>
         <v>1991</v>
       </c>
       <c r="AE3" s="3">
-        <f>AD3+1</f>
+        <f t="shared" si="0"/>
         <v>1992</v>
       </c>
       <c r="AF3" s="3">
-        <f>AE3+1</f>
+        <f t="shared" si="0"/>
         <v>1993</v>
       </c>
       <c r="AG3" s="3">
-        <f>AF3+1</f>
+        <f t="shared" si="0"/>
         <v>1994</v>
       </c>
       <c r="AH3" s="3">
-        <f>AG3+1</f>
+        <f t="shared" si="0"/>
         <v>1995</v>
       </c>
     </row>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <f t="shared" ref="A5:A35" si="0">A4+1</f>
+        <f t="shared" ref="A5:A35" si="1">A4+1</f>
         <v>1965</v>
       </c>
       <c r="P5" s="3">
@@ -2585,13 +2585,13 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1966</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1967</v>
       </c>
       <c r="N7" s="3">
@@ -2600,7 +2600,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1968</v>
       </c>
       <c r="M8" s="3">
@@ -2612,7 +2612,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1969</v>
       </c>
       <c r="L9" s="3">
@@ -2624,7 +2624,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1970</v>
       </c>
       <c r="K10" s="3">
@@ -2651,7 +2651,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1971</v>
       </c>
       <c r="J11" s="3">
@@ -2690,7 +2690,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1972</v>
       </c>
       <c r="B12" s="4"/>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1973</v>
       </c>
       <c r="B13" s="4"/>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1974</v>
       </c>
       <c r="B14" s="4"/>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1975</v>
       </c>
       <c r="B15" s="4"/>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1976</v>
       </c>
       <c r="B16" s="4"/>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1977</v>
       </c>
       <c r="B17" s="4"/>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1978</v>
       </c>
       <c r="B18" s="4"/>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1979</v>
       </c>
       <c r="B19" s="4"/>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1980</v>
       </c>
       <c r="B20" s="4"/>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1981</v>
       </c>
       <c r="B21" s="4"/>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1982</v>
       </c>
       <c r="B22" s="4"/>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1983</v>
       </c>
       <c r="B23" s="4"/>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1984</v>
       </c>
       <c r="B24" s="4"/>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1985</v>
       </c>
       <c r="B25" s="4"/>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1986</v>
       </c>
       <c r="B26" s="4"/>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1987</v>
       </c>
       <c r="B27" s="4"/>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1988</v>
       </c>
       <c r="B28" s="4"/>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1989</v>
       </c>
       <c r="B29" s="4"/>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1990</v>
       </c>
       <c r="B30" s="4"/>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
       <c r="B31" s="4"/>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1992</v>
       </c>
       <c r="B32" s="4"/>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1993</v>
       </c>
       <c r="B33" s="4"/>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1994</v>
       </c>
       <c r="B34" s="4"/>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1995</v>
       </c>
       <c r="B35" s="4"/>
@@ -3670,7 +3670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80C7F9E-393E-0949-9322-8F861CCB9A2B}">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -9851,8 +9851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5B731E-4C3A-8F4F-A603-EE25F9E67141}">
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19710,7 +19710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F9F421-4085-D148-B5A0-530C7EB0692A}">
   <dimension ref="A1:V156"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>

</xml_diff>